<commit_message>
Leaf dunk and succulence
Preliminary analysis of leaf dunk, leaf succulence data. Merge leaf surface data with leaf area. Plot as function of ecotype. Fit nested ANOVAs.
</commit_message>
<xml_diff>
--- a/Data/leaf_area_data.xlsx
+++ b/Data/leaf_area_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/plunkert_msu_edu/Documents/Leaf surfaces CP IA Images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madisonplunkert/Documents/GitHub/Leaf-surface-traits-2024/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="493" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E75B0D0-E494-1842-9AC2-6540B0AAF486}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6165A0-5BBA-A940-8981-E3CB8FEFDC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="740" windowWidth="29160" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="740" windowWidth="29160" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="16">
   <si>
     <t>pop_code</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>OAE</t>
-  </si>
-  <si>
-    <t>BHC</t>
   </si>
   <si>
     <t>HEC</t>
@@ -145,10 +142,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -470,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="291" workbookViewId="0">
-      <selection activeCell="C147" sqref="C147"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="230" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -867,7 +860,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B36">
         <v>4</v>
@@ -878,7 +871,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37">
         <v>5</v>
@@ -900,7 +893,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -922,7 +915,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B41">
         <v>15</v>
@@ -944,7 +937,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B43">
         <v>5</v>
@@ -955,7 +948,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B44">
         <v>10</v>
@@ -977,7 +970,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -988,7 +981,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47">
         <v>3</v>
@@ -1021,7 +1014,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B50">
         <v>7</v>
@@ -1032,7 +1025,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B51">
         <v>9</v>
@@ -1131,7 +1124,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B60">
         <v>12</v>
@@ -1186,7 +1179,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B65">
         <v>8</v>
@@ -1197,7 +1190,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B66">
         <v>6</v>
@@ -1219,7 +1212,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B68">
         <v>13</v>
@@ -1285,7 +1278,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B74">
         <v>6</v>
@@ -1296,7 +1289,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B75">
         <v>4</v>
@@ -1307,7 +1300,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B76">
         <v>11</v>
@@ -1318,7 +1311,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B77">
         <v>15</v>
@@ -1340,7 +1333,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -1351,7 +1344,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B80">
         <v>3</v>
@@ -1362,7 +1355,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B81">
         <v>4</v>
@@ -1384,7 +1377,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B83">
         <v>14</v>
@@ -1406,7 +1399,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B85">
         <v>11</v>
@@ -1417,7 +1410,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -1428,7 +1421,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B87">
         <v>10</v>
@@ -1439,7 +1432,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B88">
         <v>3</v>
@@ -1450,7 +1443,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B89">
         <v>10</v>
@@ -1461,7 +1454,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B90">
         <v>13</v>
@@ -1472,7 +1465,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B91">
         <v>4</v>
@@ -1483,7 +1476,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B92">
         <v>5</v>
@@ -1494,7 +1487,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B93">
         <v>15</v>
@@ -1505,7 +1498,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B94">
         <v>2</v>
@@ -1516,7 +1509,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B95">
         <v>11</v>
@@ -1527,7 +1520,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B96">
         <v>9</v>
@@ -1538,7 +1531,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B97">
         <v>6</v>
@@ -1549,7 +1542,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B98">
         <v>7</v>
@@ -1560,7 +1553,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B99">
         <v>13</v>
@@ -1571,7 +1564,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B100">
         <v>12</v>
@@ -1582,7 +1575,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B101">
         <v>5</v>
@@ -1593,7 +1586,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B102">
         <v>9</v>
@@ -1604,7 +1597,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -1615,7 +1608,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B104">
         <v>7</v>
@@ -1626,7 +1619,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B105">
         <v>8</v>
@@ -1637,7 +1630,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B106">
         <v>2</v>
@@ -1648,7 +1641,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B107">
         <v>14</v>
@@ -1659,7 +1652,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B108">
         <v>9</v>
@@ -1670,7 +1663,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B109">
         <v>8</v>
@@ -1681,7 +1674,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B110">
         <v>12</v>
@@ -1692,7 +1685,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B111">
         <v>14</v>
@@ -1703,7 +1696,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B112">
         <v>6</v>
@@ -1714,7 +1707,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B113">
         <v>11</v>
@@ -1725,7 +1718,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B114">
         <v>3</v>
@@ -1747,7 +1740,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B116">
         <v>3</v>
@@ -1758,7 +1751,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B117">
         <v>4</v>
@@ -1769,7 +1762,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B118">
         <v>13</v>
@@ -1780,7 +1773,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B119">
         <v>1</v>
@@ -1802,7 +1795,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B121">
         <v>10</v>
@@ -1813,7 +1806,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B122">
         <v>2</v>
@@ -1824,7 +1817,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B123">
         <v>2</v>
@@ -1835,7 +1828,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B124">
         <v>3</v>
@@ -1846,7 +1839,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B125">
         <v>11</v>
@@ -1857,7 +1850,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B126">
         <v>4</v>
@@ -1879,7 +1872,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B128">
         <v>14</v>
@@ -1901,7 +1894,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B130">
         <v>15</v>
@@ -1912,7 +1905,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B131">
         <v>14</v>
@@ -1923,7 +1916,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B132">
         <v>6</v>
@@ -1934,7 +1927,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B133">
         <v>7</v>
@@ -1945,7 +1938,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B134">
         <v>12</v>
@@ -1956,7 +1949,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B135">
         <v>10</v>
@@ -1989,7 +1982,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B138">
         <v>5</v>
@@ -2000,7 +1993,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B139">
         <v>9</v>
@@ -2011,7 +2004,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B140">
         <v>13</v>

</xml_diff>

<commit_message>
Metadata columns in data files to be published
</commit_message>
<xml_diff>
--- a/Data/leaf_area_data.xlsx
+++ b/Data/leaf_area_data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11003"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madisonplunkert/Documents/GitHub/Leaf-surface-traits-2024/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6165A0-5BBA-A940-8981-E3CB8FEFDC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504D07AF-6983-BA4B-8191-EAEEF883F6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="740" windowWidth="29160" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="740" windowWidth="29160" windowHeight="16920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="21">
   <si>
     <t>pop_code</t>
   </si>
@@ -84,6 +85,21 @@
   </si>
   <si>
     <t>PGR</t>
+  </si>
+  <si>
+    <t>Column Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Three-letter code for accession used</t>
+  </si>
+  <si>
+    <t>Replicate, corresponding to a separate plant from which one leaf was measured</t>
+  </si>
+  <si>
+    <t>Leaf area in cm^2 from scans taken on a document scanner and manually measured in ImageJ. Leaves were used in leaf water drop adhesion assay, succulence measurement</t>
   </si>
 </sst>
 </file>
@@ -463,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="230" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView zoomScale="230" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2082,4 +2098,51 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F4762B-6258-D742-A95A-C70AF244A2E0}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>